<commit_message>
handle duplicate matched case and add some logs
</commit_message>
<xml_diff>
--- a/src/main/resources/XMU/Order.xlsx
+++ b/src/main/resources/XMU/Order.xlsx
@@ -383,20 +383,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="SheetJS"/>
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" customWidth="true" width="20.83203125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="6.83203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.83203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="207.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="144.83203125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="13.83203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.83203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.83203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.83203125" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="8.83203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="5.83203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="6.83203125" collapsed="true"/>
     <col min="10" max="10" customWidth="true" width="8.83203125" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="8.83203125" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="24.83203125" collapsed="true"/>
@@ -442,121 +442,121 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>PO202107060946100017</v>
+        <v>PO202203231724001514</v>
       </c>
       <c r="B2" t="str">
-        <v>向宇轩</v>
+        <v>吴丽雯</v>
       </c>
       <c r="C2" t="str">
-        <v>RG01283-杨勇</v>
+        <v>RG02139-方宁</v>
       </c>
       <c r="D2" t="str">
-        <v>碳酸乙烯酯-13C3</v>
+        <v>Corning? 盖玻片CORNING(R) COVER GLASS, NO. 1 1/2, BORO&amp;</v>
       </c>
       <c r="E2" t="str">
-        <v>TM210903-0233</v>
+        <v>TM220713-0501</v>
       </c>
       <c r="F2" t="str">
-        <v>570052-1g</v>
+        <v>CLS285018-2000EA</v>
       </c>
       <c r="G2" t="str">
-        <v>1g</v>
+        <v>2000.000G</v>
       </c>
       <c r="H2" t="str">
-        <v>13200.00</v>
+        <v>520.22</v>
       </c>
       <c r="I2" t="str">
         <v>1.00</v>
       </c>
       <c r="J2" t="str">
-        <v>13200.00</v>
+        <v>520.22</v>
       </c>
       <c r="K2" t="str">
-        <v>瓶</v>
+        <v>EA</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>PO202107060946100017</v>
+        <v>PO202204181038559110</v>
       </c>
       <c r="B3" t="str">
-        <v>向宇轩</v>
+        <v>黄香菇</v>
       </c>
       <c r="C3" t="str">
-        <v>RG01283-杨勇</v>
+        <v>RG00901-夏宁邵</v>
       </c>
       <c r="D3" t="str">
-        <v>碳酸乙烯酯-d4</v>
+        <v>羟乙基哌嗪乙硫磺酸HEPES</v>
       </c>
       <c r="E3" t="str">
-        <v>TM210903-0165</v>
+        <v>TM220620-0298</v>
       </c>
       <c r="F3" t="str">
-        <v>573019-1g</v>
+        <v>H3375-1KG</v>
       </c>
       <c r="G3" t="str">
-        <v>1g</v>
+        <v>1.000KG</v>
       </c>
       <c r="H3" t="str">
-        <v>6050.00</v>
+        <v>5997.53</v>
       </c>
       <c r="I3" t="str">
         <v>1.00</v>
       </c>
       <c r="J3" t="str">
-        <v>6050.00</v>
+        <v>5997.53</v>
       </c>
       <c r="K3" t="str">
-        <v>瓶</v>
+        <v>KG</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>PO202109162132343014</v>
+        <v>PO202204181038559110</v>
       </c>
       <c r="B4" t="str">
-        <v>吴丹丹</v>
+        <v>黄香菇</v>
       </c>
       <c r="C4" t="str">
-        <v>RG00892-张晓坤</v>
+        <v>RG00901-夏宁邵</v>
       </c>
       <c r="D4" t="str">
-        <v>L-Glutathione reduced</v>
+        <v>二乙胺乙基葡聚糖 盐酸盐DEAE-DEXTRAN HYDROCHLORIDE</v>
       </c>
       <c r="E4" t="str">
-        <v>TM210923-0115</v>
+        <v>TM220620-0296</v>
       </c>
       <c r="F4" t="str">
-        <v>G4251-25G</v>
+        <v>D9885-10G</v>
       </c>
       <c r="G4" t="str">
-        <v>25G</v>
+        <v>10.000G</v>
       </c>
       <c r="H4" t="str">
-        <v>1257.72</v>
+        <v>551.88</v>
       </c>
       <c r="I4" t="str">
         <v>1.00</v>
       </c>
       <c r="J4" t="str">
-        <v>1257.72</v>
+        <v>551.88</v>
       </c>
       <c r="K4" t="str">
         <v>G</v>
       </c>
       <c r="L4" t="str">
-        <v>与官网同步</v>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204181038559110</v>
       </c>
       <c r="B5" t="str">
         <v>黄香菇</v>
@@ -565,28 +565,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D5" t="str">
-        <v>琼脂糖AGAROSE TYPE IX-A: ULTRA-LOW GELLING TE&amp;amp;</v>
+        <v>肝素酶 I 和 III 混合物 来源于肝素黄杆菌HEPARINASE I AND III BLEND FROM FLAVOBA&amp;amp;</v>
       </c>
       <c r="E5" t="str">
-        <v>TM210818-0348</v>
+        <v>TM220620-0296</v>
       </c>
       <c r="F5" t="str">
-        <v>A2576-25G</v>
+        <v>H3917-100UN</v>
       </c>
       <c r="G5" t="str">
-        <v>25.000G</v>
+        <v>100.000MG</v>
       </c>
       <c r="H5" t="str">
-        <v>2927.86</v>
+        <v>3478.67</v>
       </c>
       <c r="I5" t="str">
         <v>1.00</v>
       </c>
       <c r="J5" t="str">
-        <v>2927.86</v>
+        <v>3478.67</v>
       </c>
       <c r="K5" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L5" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204181038559110</v>
       </c>
       <c r="B6" t="str">
         <v>黄香菇</v>
@@ -603,25 +603,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D6" t="str">
-        <v>IGEPAL CA-630 MOLECULAR BIOLOGY GRADE</v>
+        <v>抗-FLAG? M2亲和凝胶ANTI-FLAG M2 AFFINITY GEL</v>
       </c>
       <c r="E6" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0296</v>
       </c>
       <c r="F6" t="str">
-        <v>I8896-50ML</v>
+        <v>A2220-5ML</v>
       </c>
       <c r="G6" t="str">
-        <v>53.000G</v>
+        <v>5.000G</v>
       </c>
       <c r="H6" t="str">
-        <v>513.12</v>
+        <v>13955.95</v>
       </c>
       <c r="I6" t="str">
         <v>1.00</v>
       </c>
       <c r="J6" t="str">
-        <v>513.12</v>
+        <v>13955.95</v>
       </c>
       <c r="K6" t="str">
         <v>ML</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202111191455194011</v>
       </c>
       <c r="B7" t="str">
         <v>黄香菇</v>
@@ -641,28 +641,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D7" t="str">
-        <v>氯化铯CESIUM CHLORIDE, FOR MOLECULAR BIOLOGY</v>
+        <v>弹性蛋白酶 来源于猪胰腺ELASTASE TYPE IV FROM PORCINE PANCREAS</v>
       </c>
       <c r="E7" t="str">
-        <v>TM210818-0350</v>
+        <v>TM211122-0405</v>
       </c>
       <c r="F7" t="str">
-        <v>C4036-1KG</v>
+        <v>E0258-20MG</v>
       </c>
       <c r="G7" t="str">
-        <v>1.000KG</v>
+        <v>20.000MG</v>
       </c>
       <c r="H7" t="str">
-        <v>4961.05</v>
+        <v>4164.28</v>
       </c>
       <c r="I7" t="str">
         <v>1.00</v>
       </c>
       <c r="J7" t="str">
-        <v>4961.05</v>
+        <v>4164.28</v>
       </c>
       <c r="K7" t="str">
-        <v>KG</v>
+        <v>MG</v>
       </c>
       <c r="L7" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204201709004020</v>
       </c>
       <c r="B8" t="str">
         <v>黄香菇</v>
@@ -679,25 +679,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D8" t="str">
-        <v>转铁蛋白 人TRANSFERRIN HUMAN PARTIALLY IRON- SATURA</v>
+        <v>D-(?)-3-磷酸甘油酸 二钠盐D(-)3-PHOSPHOGLYCERIC ACID DISODIUM</v>
       </c>
       <c r="E8" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0306</v>
       </c>
       <c r="F8" t="str">
-        <v>T8158-100MG</v>
+        <v>P8877-10MG</v>
       </c>
       <c r="G8" t="str">
-        <v>100.000MG</v>
+        <v>10.000MG</v>
       </c>
       <c r="H8" t="str">
-        <v>1019.96</v>
+        <v>181.97</v>
       </c>
       <c r="I8" t="str">
-        <v>1.00</v>
+        <v>10.00</v>
       </c>
       <c r="J8" t="str">
-        <v>1019.96</v>
+        <v>1819.70</v>
       </c>
       <c r="K8" t="str">
         <v>MG</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204201709004020</v>
       </c>
       <c r="B9" t="str">
         <v>黄香菇</v>
@@ -717,25 +717,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D9" t="str">
-        <v>重组人表皮细胞生长因子EPIDERMAL GROWTH FACTOR HUMAN, EGF&amp;amp;</v>
+        <v>羟基丙酮酸磷酸酯 锂盐HYDROXYPYRUVIC ACID PHOSPHATE LITHIUM S&amp;amp;</v>
       </c>
       <c r="E9" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0305</v>
       </c>
       <c r="F9" t="str">
-        <v>E9644-.5MG</v>
+        <v>02711-10MG</v>
       </c>
       <c r="G9" t="str">
-        <v>0.500MG</v>
+        <v>10.000MG</v>
       </c>
       <c r="H9" t="str">
-        <v>3387.11</v>
+        <v>795.28</v>
       </c>
       <c r="I9" t="str">
         <v>1.00</v>
       </c>
       <c r="J9" t="str">
-        <v>3387.11</v>
+        <v>795.28</v>
       </c>
       <c r="K9" t="str">
         <v>MG</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202108171046304011</v>
       </c>
       <c r="B10" t="str">
         <v>黄香菇</v>
@@ -755,36 +755,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D10" t="str">
-        <v>Aprotinin</v>
+        <v>N-ACETYL-ALPHA-D-GLUCOSAMINE 1-PHOS&amp;amp;</v>
       </c>
       <c r="E10" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0265</v>
       </c>
       <c r="F10" t="str">
-        <v>10236624001</v>
+        <v>A2142-5MG</v>
       </c>
       <c r="G10" t="str">
-        <v>1EA</v>
+        <v>5.000MG</v>
       </c>
       <c r="H10" t="str">
-        <v>743.61</v>
+        <v>451.70</v>
       </c>
       <c r="I10" t="str">
         <v>1.00</v>
       </c>
       <c r="J10" t="str">
-        <v>743.61</v>
+        <v>451.70</v>
       </c>
       <c r="K10" t="str">
-        <v>EA</v>
+        <v>MG</v>
       </c>
       <c r="L10" t="str">
-        <v>与官网同步</v>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202203161106574015</v>
       </c>
       <c r="B11" t="str">
         <v>黄香菇</v>
@@ -793,74 +793,74 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D11" t="str">
-        <v>Leupeptin</v>
+        <v>杜氏改良 Eagle 培养基 - 高葡萄糖DULBECCOS MODIFIED EAGLES MEDIUM - HIG</v>
       </c>
       <c r="E11" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220606-0501</v>
       </c>
       <c r="F11" t="str">
-        <v>11017101001</v>
+        <v>D6429-500ML</v>
       </c>
       <c r="G11" t="str">
-        <v>1EA</v>
+        <v>500.000G</v>
       </c>
       <c r="H11" t="str">
-        <v>946.99</v>
+        <v>41.00</v>
       </c>
       <c r="I11" t="str">
-        <v>1.00</v>
+        <v>400.00</v>
       </c>
       <c r="J11" t="str">
-        <v>946.99</v>
+        <v>16400.00</v>
       </c>
       <c r="K11" t="str">
-        <v>EA</v>
+        <v>ML</v>
       </c>
       <c r="L11" t="str">
-        <v>与官网同步</v>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>PO202107060946100017</v>
+        <v>PO202204191310119119</v>
       </c>
       <c r="B12" t="str">
-        <v>向宇轩</v>
+        <v>陈毅歆</v>
       </c>
       <c r="C12" t="str">
-        <v>RG01283-杨勇</v>
+        <v>RG00901-夏宁邵</v>
       </c>
       <c r="D12" t="str">
-        <v>碳酸乙烯酯-13C</v>
+        <v>吸头PIPETTE TIPS, 200 UL, YELLOW</v>
       </c>
       <c r="E12" t="str">
-        <v>TM210903-0165</v>
+        <v>TM220712-0258</v>
       </c>
       <c r="F12" t="str">
-        <v>658634-1g</v>
+        <v>AXYT200Y</v>
       </c>
       <c r="G12" t="str">
-        <v>1g</v>
+        <v>6360.300G</v>
       </c>
       <c r="H12" t="str">
-        <v>12500.00</v>
+        <v>1247.40</v>
       </c>
       <c r="I12" t="str">
         <v>1.00</v>
       </c>
       <c r="J12" t="str">
-        <v>12500.00</v>
+        <v>1247.40</v>
       </c>
       <c r="K12" t="str">
-        <v>瓶</v>
+        <v>EA</v>
       </c>
       <c r="L12" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204181038559110</v>
       </c>
       <c r="B13" t="str">
         <v>黄香菇</v>
@@ -869,28 +869,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D13" t="str">
-        <v>弹性蛋白酶 来源于猪胰腺ELASTASE TYPE IV FROM PORCINE PANCREAS</v>
+        <v>SSYPRO? Orange蛋白凝胶染色剂SYPRO ORANGE PROTEIN GEL STAIN</v>
       </c>
       <c r="E13" t="str">
-        <v>TM210818-0348</v>
+        <v>TM220620-0296</v>
       </c>
       <c r="F13" t="str">
-        <v>E0258-10MG</v>
+        <v>S5692-500UL</v>
       </c>
       <c r="G13" t="str">
-        <v>10.000MG</v>
+        <v>550.000MG</v>
       </c>
       <c r="H13" t="str">
-        <v>2244.09</v>
+        <v>2142.16</v>
       </c>
       <c r="I13" t="str">
         <v>1.00</v>
       </c>
       <c r="J13" t="str">
-        <v>2244.09</v>
+        <v>2142.16</v>
       </c>
       <c r="K13" t="str">
-        <v>MG</v>
+        <v>EA</v>
       </c>
       <c r="L13" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205171244564010</v>
       </c>
       <c r="B14" t="str">
         <v>黄香菇</v>
@@ -907,25 +907,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D14" t="str">
-        <v>N-EPSILON-2-4-DNP-L-LYSINE HYDROCHLORIDE</v>
+        <v>磷酸肌酸 二钠盐 水合物PHOSPHOCREATINE DISODIUM HYDRATE</v>
       </c>
       <c r="E14" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0401</v>
       </c>
       <c r="F14" t="str">
-        <v>D0380-1G</v>
+        <v>P7936-1G</v>
       </c>
       <c r="G14" t="str">
         <v>1.000G</v>
       </c>
       <c r="H14" t="str">
-        <v>993.88</v>
+        <v>840.37</v>
       </c>
       <c r="I14" t="str">
         <v>1.00</v>
       </c>
       <c r="J14" t="str">
-        <v>993.88</v>
+        <v>840.37</v>
       </c>
       <c r="K14" t="str">
         <v>G</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205171244564010</v>
       </c>
       <c r="B15" t="str">
         <v>黄香菇</v>
@@ -945,36 +945,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D15" t="str">
-        <v>D-(+)-海藻糖 二水合物D(+)TREHALOSE REDUCED METAL ION CONTENT&amp;amp;</v>
+        <v>脱氧核糖核酸 钠盐</v>
       </c>
       <c r="E15" t="str">
-        <v>TM210810-0163</v>
+        <v>TM220620-0399</v>
       </c>
       <c r="F15" t="str">
-        <v>T9531-100G</v>
+        <v>D1626-1g</v>
       </c>
       <c r="G15" t="str">
-        <v>100.000G</v>
+        <v>1g</v>
       </c>
       <c r="H15" t="str">
-        <v>6636.74</v>
+        <v>1253.95</v>
       </c>
       <c r="I15" t="str">
         <v>1.00</v>
       </c>
       <c r="J15" t="str">
-        <v>6636.74</v>
+        <v>1253.95</v>
       </c>
       <c r="K15" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L15" t="str">
-        <v>现货一周内，期货咨询销售</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205171244564010</v>
       </c>
       <c r="B16" t="str">
         <v>黄香菇</v>
@@ -983,28 +983,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D16" t="str">
-        <v>葡聚糖 来源于明串珠菌 属DEXTRAN FROM LEUCONOSTOC SSP.&amp;amp;</v>
+        <v>Dispase II (neutral protease, grade II)酶DispaseSUP?/SUP II (neutral protease, grade II)</v>
       </c>
       <c r="E16" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220620-0399</v>
       </c>
       <c r="F16" t="str">
-        <v>31389-100G</v>
+        <v>4942078001</v>
       </c>
       <c r="G16" t="str">
-        <v>100.000G</v>
+        <v>1EA</v>
       </c>
       <c r="H16" t="str">
-        <v>3009.56</v>
+        <v>6172.17</v>
       </c>
       <c r="I16" t="str">
         <v>1.00</v>
       </c>
       <c r="J16" t="str">
-        <v>3009.56</v>
+        <v>6172.17</v>
       </c>
       <c r="K16" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L16" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1012,37 +1012,37 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204191310119119</v>
       </c>
       <c r="B17" t="str">
-        <v>黄香菇</v>
+        <v>陈毅歆</v>
       </c>
       <c r="C17" t="str">
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D17" t="str">
-        <v>抗-FLAG? M2亲和凝胶ANTI-FLAG M2 AFFINITY GEL</v>
+        <v>SCREW CAPS WITH O-RINGS, WHITE</v>
       </c>
       <c r="E17" t="str">
-        <v>TM210818-0350</v>
+        <v>TM220712-0262</v>
       </c>
       <c r="F17" t="str">
-        <v>A2220-1ML</v>
+        <v>AXYSCOW</v>
       </c>
       <c r="G17" t="str">
-        <v>1.000G</v>
+        <v>2.500KG</v>
       </c>
       <c r="H17" t="str">
-        <v>5486.72</v>
+        <v>1851.07</v>
       </c>
       <c r="I17" t="str">
-        <v>2.00</v>
+        <v>7.00</v>
       </c>
       <c r="J17" t="str">
-        <v>10973.44</v>
+        <v>12957.49</v>
       </c>
       <c r="K17" t="str">
-        <v>ML</v>
+        <v>EA</v>
       </c>
       <c r="L17" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1050,37 +1050,37 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202204191310119119</v>
       </c>
       <c r="B18" t="str">
-        <v>黄香菇</v>
+        <v>陈毅歆</v>
       </c>
       <c r="C18" t="str">
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D18" t="str">
-        <v>诺布尔琼脂NOBLE AGAR</v>
+        <v>Corning? Transwell? 聚碳酸酯膜细胞培养插入物CORNING(R) TRANSWELL(R) POLYCARBONATE M&amp;amp;</v>
       </c>
       <c r="E18" t="str">
-        <v>TM210818-0348</v>
+        <v>TM220620-0383</v>
       </c>
       <c r="F18" t="str">
-        <v>A5431-250G</v>
+        <v>CLS3413-48EA</v>
       </c>
       <c r="G18" t="str">
-        <v>250.000G</v>
+        <v>48.000G</v>
       </c>
       <c r="H18" t="str">
-        <v>3375.32</v>
+        <v>1197.07</v>
       </c>
       <c r="I18" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J18" t="str">
-        <v>3375.32</v>
+        <v>2394.14</v>
       </c>
       <c r="K18" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L18" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205171244564010</v>
       </c>
       <c r="B19" t="str">
         <v>黄香菇</v>
@@ -1097,28 +1097,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D19" t="str">
-        <v>胃蛋白酶 来源于猪胃粘膜PEPSIN FROM PORCINE GASTRIC MUCOSA</v>
+        <v>DL-二硫代苏糖醇 溶液DL-DITHIOTHREITOL SOLUTION, BIOULTRA, FO</v>
       </c>
       <c r="E19" t="str">
-        <v>TM210818-0348</v>
+        <v>TM220620-0407</v>
       </c>
       <c r="F19" t="str">
-        <v>P6887-250MG</v>
+        <v>43816-10ML</v>
       </c>
       <c r="G19" t="str">
-        <v>250.000MG</v>
+        <v>10.400G</v>
       </c>
       <c r="H19" t="str">
-        <v>612.95</v>
+        <v>332.28</v>
       </c>
       <c r="I19" t="str">
-        <v>6.00</v>
+        <v>1.00</v>
       </c>
       <c r="J19" t="str">
-        <v>3677.70</v>
+        <v>332.28</v>
       </c>
       <c r="K19" t="str">
-        <v>MG</v>
+        <v>ML</v>
       </c>
       <c r="L19" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205191300544013</v>
       </c>
       <c r="B20" t="str">
         <v>黄香菇</v>
@@ -1135,36 +1135,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D20" t="str">
-        <v>十二烷基硫酸钠An ionic detergent useful in electrophoretic separation of proteins and lipids.</v>
+        <v>X-tremeGENESUP?/SUP HP DNA转染试剂X-tremeGENE(TM) HP DNA Transfection Reagent</v>
       </c>
       <c r="E20" t="str">
-        <v>TM210810-0164</v>
+        <v>TM220620-0412</v>
       </c>
       <c r="F20" t="str">
-        <v>428015-1KG</v>
+        <v>6366546001</v>
       </c>
       <c r="G20" t="str">
-        <v>1KG</v>
+        <v>1EA</v>
       </c>
       <c r="H20" t="str">
-        <v>1578.05</v>
+        <v>24743.44</v>
       </c>
       <c r="I20" t="str">
-        <v>5.00</v>
+        <v>1.00</v>
       </c>
       <c r="J20" t="str">
-        <v>7890.25</v>
+        <v>24743.44</v>
       </c>
       <c r="K20" t="str">
         <v>EA</v>
       </c>
       <c r="L20" t="str">
-        <v>与官网同步</v>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>PO202108061529554014</v>
+        <v>PO202205191300544013</v>
       </c>
       <c r="B21" t="str">
         <v>黄香菇</v>
@@ -1173,28 +1173,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D21" t="str">
-        <v>cOmplete(TM), EDTA-free Protease Inhibitor Cocktail抗体Roche cOmpleteSUP?/SUP Protease Inhibitor Cocktail EDTA-free tablets contain an optimized mix of protease inhibitors to inhibit a broad range of proteases</v>
+        <v>杜氏改良 Eagle 培养基 - 高葡萄糖DULBECCOS MODIFIED EAGLES MEDIUM - HIG</v>
       </c>
       <c r="E21" t="str">
-        <v>TM210818-0348</v>
+        <v>TM220606-0492</v>
       </c>
       <c r="F21" t="str">
-        <v>4693132001</v>
+        <v>D6429-500ML</v>
       </c>
       <c r="G21" t="str">
-        <v>1EA</v>
+        <v>500.000G</v>
       </c>
       <c r="H21" t="str">
-        <v>3381.92</v>
+        <v>41.00</v>
       </c>
       <c r="I21" t="str">
-        <v>1.00</v>
+        <v>32.00</v>
       </c>
       <c r="J21" t="str">
-        <v>3381.92</v>
+        <v>1312.00</v>
       </c>
       <c r="K21" t="str">
-        <v>EA</v>
+        <v>ML</v>
       </c>
       <c r="L21" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202205191300544013</v>
       </c>
       <c r="B22" t="str">
         <v>黄香菇</v>
@@ -1211,28 +1211,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D22" t="str">
-        <v>环亮氨酸1-AMINO-1-CYCLOPENTANECARBOXYLIC ACID, &amp;amp;</v>
+        <v>MPLA (PHAD (R))</v>
       </c>
       <c r="E22" t="str">
-        <v>TM210906-0389</v>
+        <v>TM220620-0410</v>
       </c>
       <c r="F22" t="str">
-        <v>A48105-5G</v>
+        <v>699800P-5MG</v>
       </c>
       <c r="G22" t="str">
-        <v>5.000G</v>
+        <v>5.000MG</v>
       </c>
       <c r="H22" t="str">
-        <v>1348.06</v>
+        <v>6876.05</v>
       </c>
       <c r="I22" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J22" t="str">
-        <v>1348.06</v>
+        <v>13752.10</v>
       </c>
       <c r="K22" t="str">
-        <v>G</v>
+        <v>MG</v>
       </c>
       <c r="L22" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B23" t="str">
         <v>黄香菇</v>
@@ -1249,28 +1249,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D23" t="str">
-        <v>乙酰乙酸锂LITHIUM ACETOACETATE =90% (HPLC)</v>
+        <v>PERCOLL CELL CULTURE TESTED</v>
       </c>
       <c r="E23" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220620-0417</v>
       </c>
       <c r="F23" t="str">
-        <v>A8509-10MG</v>
+        <v>P4937-500ML</v>
       </c>
       <c r="G23" t="str">
-        <v>10.000MG</v>
+        <v>565.000G</v>
       </c>
       <c r="H23" t="str">
-        <v>334.89</v>
+        <v>4998.07</v>
       </c>
       <c r="I23" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J23" t="str">
-        <v>334.89</v>
+        <v>9996.14</v>
       </c>
       <c r="K23" t="str">
-        <v>MG</v>
+        <v>ML</v>
       </c>
       <c r="L23" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B24" t="str">
         <v>黄香菇</v>
@@ -1287,25 +1287,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D24" t="str">
-        <v>4-甲基-2-氧戊酸4-Methyl-2-oxovaleric acid, = 98.0 % T&amp;amp;</v>
+        <v>d-脱硫生物素D-DESTHIOBIOTIN</v>
       </c>
       <c r="E24" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220712-0263</v>
       </c>
       <c r="F24" t="str">
-        <v>68255-1G</v>
+        <v>D1411-1G</v>
       </c>
       <c r="G24" t="str">
         <v>1.000G</v>
       </c>
       <c r="H24" t="str">
-        <v>664.09</v>
+        <v>2410.40</v>
       </c>
       <c r="I24" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J24" t="str">
-        <v>664.09</v>
+        <v>4820.80</v>
       </c>
       <c r="K24" t="str">
         <v>G</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B25" t="str">
         <v>黄香菇</v>
@@ -1325,28 +1325,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D25" t="str">
-        <v>2′-脱氧腺苷-5′-单磷酸2-DEOXYADENOSINE 5-MONOPHOSPHATE FREE</v>
+        <v>丁酸钠SODIUM BUTYRATE</v>
       </c>
       <c r="E25" t="str">
-        <v>TM210906-0389</v>
+        <v>TM220712-0264</v>
       </c>
       <c r="F25" t="str">
-        <v>D6375-100MG</v>
+        <v>B5887-5G</v>
       </c>
       <c r="G25" t="str">
-        <v>100.000MG</v>
+        <v>5.000G</v>
       </c>
       <c r="H25" t="str">
-        <v>402.49</v>
+        <v>2963.03</v>
       </c>
       <c r="I25" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J25" t="str">
-        <v>402.49</v>
+        <v>5926.06</v>
       </c>
       <c r="K25" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L25" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1354,7 +1354,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B26" t="str">
         <v>黄香菇</v>
@@ -1363,28 +1363,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D26" t="str">
-        <v>DL-DIHYDROOROTIC ACID</v>
+        <v>视黄酸RETINOIC ACID</v>
       </c>
       <c r="E26" t="str">
-        <v>TM210906-0389</v>
+        <v>TM220712-0267</v>
       </c>
       <c r="F26" t="str">
-        <v>D7003-100MG</v>
+        <v>R2625-1G</v>
       </c>
       <c r="G26" t="str">
-        <v>100.000MG</v>
+        <v>1.000G</v>
       </c>
       <c r="H26" t="str">
-        <v>645.86</v>
+        <v>1825.97</v>
       </c>
       <c r="I26" t="str">
         <v>1.00</v>
       </c>
       <c r="J26" t="str">
-        <v>645.86</v>
+        <v>1825.97</v>
       </c>
       <c r="K26" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L26" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B27" t="str">
         <v>黄香菇</v>
@@ -1401,28 +1401,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D27" t="str">
-        <v>D-葡萄糖胺6-磷酸D-GLUCOSAMINE 6-PHOSPHATE FREE ACID</v>
+        <v>生物素BIOTIN, =99% (HPLC), LYOPHILIZED POWDER</v>
       </c>
       <c r="E27" t="str">
-        <v>TM210906-0394</v>
+        <v>TM220712-0272</v>
       </c>
       <c r="F27" t="str">
-        <v>G5509-100MG</v>
+        <v>B4501-10G</v>
       </c>
       <c r="G27" t="str">
-        <v>100.000MG</v>
+        <v>10.000G</v>
       </c>
       <c r="H27" t="str">
-        <v>852.94</v>
+        <v>4755.78</v>
       </c>
       <c r="I27" t="str">
         <v>1.00</v>
       </c>
       <c r="J27" t="str">
-        <v>852.94</v>
+        <v>4755.78</v>
       </c>
       <c r="K27" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L27" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1430,7 +1430,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B28" t="str">
         <v>黄香菇</v>
@@ -1439,28 +1439,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D28" t="str">
-        <v>2,3-吡啶二甲酸2,3-PYRIDINEDICARBOXYLIC ACID, 99%</v>
+        <v>蛋白酶 K 来源于林伯氏白色念球菌Proteinase K, Tritirachium album</v>
       </c>
       <c r="E28" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220712-0274</v>
       </c>
       <c r="F28" t="str">
-        <v>P63204-25G</v>
+        <v>539480-100MG</v>
       </c>
       <c r="G28" t="str">
-        <v>25.000G</v>
+        <v>100MG</v>
       </c>
       <c r="H28" t="str">
-        <v>196.06</v>
+        <v>1262.41</v>
       </c>
       <c r="I28" t="str">
         <v>1.00</v>
       </c>
       <c r="J28" t="str">
-        <v>196.06</v>
+        <v>1262.41</v>
       </c>
       <c r="K28" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L28" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B29" t="str">
         <v>黄香菇</v>
@@ -1477,25 +1477,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D29" t="str">
-        <v>2,5-二羟基苯甲酸2,5-Dihydroxybenzoic acid, 98%</v>
+        <v>甲基纤维素METHYL CELLULOSE,  VISCOSITY 15 CP</v>
       </c>
       <c r="E29" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220620-0417</v>
       </c>
       <c r="F29" t="str">
-        <v>149357-10G</v>
+        <v>M7140-100G</v>
       </c>
       <c r="G29" t="str">
-        <v>10.000G</v>
+        <v>100.000G</v>
       </c>
       <c r="H29" t="str">
-        <v>225.77</v>
+        <v>595.10</v>
       </c>
       <c r="I29" t="str">
         <v>1.00</v>
       </c>
       <c r="J29" t="str">
-        <v>225.77</v>
+        <v>595.10</v>
       </c>
       <c r="K29" t="str">
         <v>G</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B30" t="str">
         <v>黄香菇</v>
@@ -1515,28 +1515,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D30" t="str">
-        <v>2-羟基异己酸2-HYDROXYISOCAPROIC ACID, 99%</v>
+        <v>伴刀豆球蛋白A 来源于洋刀豆 （刀豆）CONCANAVALIN A TYPE IV</v>
       </c>
       <c r="E30" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220620-0417</v>
       </c>
       <c r="F30" t="str">
-        <v>219819-1G</v>
+        <v>C2010-100MG</v>
       </c>
       <c r="G30" t="str">
-        <v>1.000G</v>
+        <v>100.000MG</v>
       </c>
       <c r="H30" t="str">
-        <v>762.85</v>
+        <v>725.93</v>
       </c>
       <c r="I30" t="str">
         <v>1.00</v>
       </c>
       <c r="J30" t="str">
-        <v>762.85</v>
+        <v>725.93</v>
       </c>
       <c r="K30" t="str">
-        <v>G</v>
+        <v>MG</v>
       </c>
       <c r="L30" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>PO202108171046304011</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B31" t="str">
         <v>黄香菇</v>
@@ -1553,36 +1553,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D31" t="str">
-        <v>ATP</v>
+        <v>三甲胺N-氧化物TRIMETHYLAMINE N-OXIDE, 95%</v>
       </c>
       <c r="E31" t="str">
-        <v>TM210819-0076</v>
+        <v>TM220620-0419</v>
       </c>
       <c r="F31" t="str">
-        <v>11140965001</v>
+        <v>317594-1G</v>
       </c>
       <c r="G31" t="str">
-        <v>400ul</v>
+        <v>1.000G</v>
       </c>
       <c r="H31" t="str">
-        <v>1065.34</v>
+        <v>535.40</v>
       </c>
       <c r="I31" t="str">
         <v>1.00</v>
       </c>
       <c r="J31" t="str">
-        <v>1065.34</v>
+        <v>535.40</v>
       </c>
       <c r="K31" t="str">
-        <v>瓶</v>
+        <v>G</v>
       </c>
       <c r="L31" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>PO202108171046304011</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B32" t="str">
         <v>黄香菇</v>
@@ -1591,36 +1591,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D32" t="str">
-        <v>L -氧化谷胱甘肽</v>
+        <v>RESOMER? RG 502 H,聚（d,L-丙交酯-共-乙交酯）RESOMER(R) RG 502 H, POLY(D,L-LACTIDE-CO</v>
       </c>
       <c r="E32" t="str">
-        <v>TM210819-0076</v>
+        <v>TM220620-0419</v>
       </c>
       <c r="F32" t="str">
-        <v>G4376-250MG</v>
+        <v>719897-5G</v>
       </c>
       <c r="G32" t="str">
-        <v>250mg</v>
+        <v>5.000G</v>
       </c>
       <c r="H32" t="str">
-        <v>461.04</v>
+        <v>2832.59</v>
       </c>
       <c r="I32" t="str">
         <v>1.00</v>
       </c>
       <c r="J32" t="str">
-        <v>461.04</v>
+        <v>2832.59</v>
       </c>
       <c r="K32" t="str">
-        <v>瓶</v>
+        <v>G</v>
       </c>
       <c r="L32" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>PO202108171046304011</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B33" t="str">
         <v>黄香菇</v>
@@ -1629,36 +1629,36 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D33" t="str">
-        <v>N-乙酰-D-甘露糖胺</v>
+        <v>杜氏改良 Eagle 培养基 - 高葡萄糖DULBECCOS MODIFIED EAGLES MEDIUM - HIG</v>
       </c>
       <c r="E33" t="str">
-        <v>TM210819-0079</v>
+        <v>TM220620-0413</v>
       </c>
       <c r="F33" t="str">
-        <v>PHG0017-10G</v>
+        <v>D6429-500ML</v>
       </c>
       <c r="G33" t="str">
-        <v>10g</v>
+        <v>500.000G</v>
       </c>
       <c r="H33" t="str">
-        <v>2404.64</v>
+        <v>41.00</v>
       </c>
       <c r="I33" t="str">
-        <v>1.00</v>
+        <v>400.00</v>
       </c>
       <c r="J33" t="str">
-        <v>2404.64</v>
+        <v>16400.00</v>
       </c>
       <c r="K33" t="str">
-        <v>瓶</v>
+        <v>ML</v>
       </c>
       <c r="L33" t="str">
-        <v/>
+        <v>现货一周内，期货咨询销售</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202205191300544013</v>
       </c>
       <c r="B34" t="str">
         <v>黄香菇</v>
@@ -1667,28 +1667,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D34" t="str">
-        <v>D-葡糖醛酸D-GLUCURONIC ACID</v>
+        <v>杜氏改良 Eagle 培养基 - 高葡萄糖DULBECCOS MODIFIED EAGLES MEDIUM - HIG</v>
       </c>
       <c r="E34" t="str">
-        <v>TM210906-0394</v>
+        <v>TM220606-0492</v>
       </c>
       <c r="F34" t="str">
-        <v>G5269-10MG</v>
+        <v>D6429-500ML</v>
       </c>
       <c r="G34" t="str">
-        <v>10.000MG</v>
+        <v>500.000G</v>
       </c>
       <c r="H34" t="str">
-        <v>239.23</v>
+        <v>41.00</v>
       </c>
       <c r="I34" t="str">
-        <v>1.00</v>
+        <v>73.00</v>
       </c>
       <c r="J34" t="str">
-        <v>239.23</v>
+        <v>2993.00</v>
       </c>
       <c r="K34" t="str">
-        <v>MG</v>
+        <v>ML</v>
       </c>
       <c r="L34" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B35" t="str">
         <v>黄香菇</v>
@@ -1705,28 +1705,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D35" t="str">
-        <v>肌苷-5′-单磷酸 二钠盐 水合物INOSINE 5-MONOPHOSPHATE DISODIUM SALT&amp;amp;</v>
+        <v>单克隆抗-FLAG?MONOCLONAL ANTI-FLAG</v>
       </c>
       <c r="E35" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220704-0403</v>
       </c>
       <c r="F35" t="str">
-        <v>I4625-5G</v>
+        <v>F2555-100UL</v>
       </c>
       <c r="G35" t="str">
-        <v>5.000G</v>
+        <v>100.000MG</v>
       </c>
       <c r="H35" t="str">
-        <v>442.18</v>
+        <v>4425.95</v>
       </c>
       <c r="I35" t="str">
         <v>1.00</v>
       </c>
       <c r="J35" t="str">
-        <v>442.18</v>
+        <v>4425.95</v>
       </c>
       <c r="K35" t="str">
-        <v>G</v>
+        <v>EA</v>
       </c>
       <c r="L35" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B36" t="str">
         <v>黄香菇</v>
@@ -1743,25 +1743,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D36" t="str">
-        <v>(±)-α-硫辛酸(+/-)-A-LIPOIC ACID, BIOREAGENT, = 99&amp;amp;</v>
+        <v>RESOMER? RG 502 H,聚（d,L-丙交酯-共-乙交酯）RESOMER(R) RG 502 H, POLY(D,L-LACTIDE-CO</v>
       </c>
       <c r="E36" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220704-0389</v>
       </c>
       <c r="F36" t="str">
-        <v>T1395-1G</v>
+        <v>719897-1G</v>
       </c>
       <c r="G36" t="str">
         <v>1.000G</v>
       </c>
       <c r="H36" t="str">
-        <v>434.05</v>
+        <v>881.14</v>
       </c>
       <c r="I36" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J36" t="str">
-        <v>434.05</v>
+        <v>1762.28</v>
       </c>
       <c r="K36" t="str">
         <v>G</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B37" t="str">
         <v>黄香菇</v>
@@ -1781,28 +1781,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D37" t="str">
-        <v>2-酮己酸 钠盐A-KETOCAPROIC ACID SODIUM</v>
+        <v>X-tremeGENESUP?/SUP HP DNA转染试剂X-tremeGENE(TM) HP DNA Transfection Reagent</v>
       </c>
       <c r="E37" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220704-0392</v>
       </c>
       <c r="F37" t="str">
-        <v>K6625-250MG</v>
+        <v>6366236001</v>
       </c>
       <c r="G37" t="str">
-        <v>250.000MG</v>
+        <v>1EA</v>
       </c>
       <c r="H37" t="str">
-        <v>3304.90</v>
+        <v>5114.66</v>
       </c>
       <c r="I37" t="str">
-        <v>1.00</v>
+        <v>10.00</v>
       </c>
       <c r="J37" t="str">
-        <v>3304.90</v>
+        <v>51146.60</v>
       </c>
       <c r="K37" t="str">
-        <v>MG</v>
+        <v>EA</v>
       </c>
       <c r="L37" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B38" t="str">
         <v>黄香菇</v>
@@ -1819,28 +1819,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D38" t="str">
-        <v>3,4-二羟基苯乙酸3,4-DIHYDROXYPHENYLACETIC ACID, 98%</v>
+        <v>D-α-生育酚琥珀酸酯A-TOCOPHERYL ACID SUCCINATE</v>
       </c>
       <c r="E38" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220704-0406</v>
       </c>
       <c r="F38" t="str">
-        <v>850217-1G</v>
+        <v>PHR1029-500MG</v>
       </c>
       <c r="G38" t="str">
-        <v>1.000G</v>
+        <v>500.000MG</v>
       </c>
       <c r="H38" t="str">
-        <v>225.77</v>
+        <v>806.44</v>
       </c>
       <c r="I38" t="str">
         <v>1.00</v>
       </c>
       <c r="J38" t="str">
-        <v>225.77</v>
+        <v>806.44</v>
       </c>
       <c r="K38" t="str">
-        <v>G</v>
+        <v>MG</v>
       </c>
       <c r="L38" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>PO202108251044194018</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B39" t="str">
         <v>黄香菇</v>
@@ -1857,25 +1857,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D39" t="str">
-        <v>D-(?)-3-磷酸甘油酸 二钠盐D(-)3-PHOSPHOGLYCERIC ACID DISODIUM</v>
+        <v>PMA, FOR USE IN MOLECULAR BIOLOGY APPLIC</v>
       </c>
       <c r="E39" t="str">
-        <v>TM210906-0393</v>
+        <v>TM220704-0407</v>
       </c>
       <c r="F39" t="str">
-        <v>P8877-10MG</v>
+        <v>P1585-1MG</v>
       </c>
       <c r="G39" t="str">
-        <v>10.000MG</v>
+        <v>1.000MG</v>
       </c>
       <c r="H39" t="str">
-        <v>164.54</v>
+        <v>1231.46</v>
       </c>
       <c r="I39" t="str">
         <v>1.00</v>
       </c>
       <c r="J39" t="str">
-        <v>164.54</v>
+        <v>1231.46</v>
       </c>
       <c r="K39" t="str">
         <v>MG</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206211147314015</v>
       </c>
       <c r="B40" t="str">
         <v>黄香菇</v>
@@ -1895,25 +1895,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D40" t="str">
-        <v>烟酸腺嘌呤二核苷酸 钠盐NICOTINIC ACID ADENINE DINUCLEOTIDE    &amp;amp;</v>
+        <v>佛波醇12-十四酸酯13-乙酸酯PHORBOL 12-MYRISTATE 13-ACETATE</v>
       </c>
       <c r="E40" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220704-0412</v>
       </c>
       <c r="F40" t="str">
-        <v>N4256-25MG</v>
+        <v>P8139-5MG</v>
       </c>
       <c r="G40" t="str">
-        <v>25.000MG</v>
+        <v>5.000MG</v>
       </c>
       <c r="H40" t="str">
-        <v>1035.23</v>
+        <v>2484.17</v>
       </c>
       <c r="I40" t="str">
         <v>1.00</v>
       </c>
       <c r="J40" t="str">
-        <v>1035.23</v>
+        <v>2484.17</v>
       </c>
       <c r="K40" t="str">
         <v>MG</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206081550084011</v>
       </c>
       <c r="B41" t="str">
         <v>黄香菇</v>
@@ -1933,28 +1933,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D41" t="str">
-        <v>Nα-乙酰基-L-鸟氨酸N-A-ACETYL-L-ORNITHINE CRYSTALLINE</v>
+        <v>DNase I酶DNase I</v>
       </c>
       <c r="E41" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220620-0417</v>
       </c>
       <c r="F41" t="str">
-        <v>A3626-500MG</v>
+        <v>11284932001</v>
       </c>
       <c r="G41" t="str">
-        <v>500.000MG</v>
+        <v>100mg</v>
       </c>
       <c r="H41" t="str">
-        <v>2169.94</v>
+        <v>1638.61</v>
       </c>
       <c r="I41" t="str">
-        <v>1.00</v>
+        <v>5.00</v>
       </c>
       <c r="J41" t="str">
-        <v>2169.94</v>
+        <v>8193.05</v>
       </c>
       <c r="K41" t="str">
-        <v>MG</v>
+        <v>EA</v>
       </c>
       <c r="L41" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -1962,7 +1962,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202204201709004020</v>
       </c>
       <c r="B42" t="str">
         <v>黄香菇</v>
@@ -1971,25 +1971,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D42" t="str">
-        <v>吡哆醛5-磷酸盐 水合物PYRIDOXAL 5-PHOSPHATE HYDRATE, =98%</v>
+        <v>硫胺素焦磷酸THIAMINE PYROPHOSPHATE, =95%</v>
       </c>
       <c r="E42" t="str">
-        <v>TM210906-0391</v>
+        <v>TM220620-0303</v>
       </c>
       <c r="F42" t="str">
-        <v>P9255-1G</v>
+        <v>C8754-1G</v>
       </c>
       <c r="G42" t="str">
         <v>1.000G</v>
       </c>
       <c r="H42" t="str">
-        <v>411.32</v>
+        <v>233.54</v>
       </c>
       <c r="I42" t="str">
         <v>1.00</v>
       </c>
       <c r="J42" t="str">
-        <v>411.32</v>
+        <v>233.54</v>
       </c>
       <c r="K42" t="str">
         <v>G</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202204201709004020</v>
       </c>
       <c r="B43" t="str">
         <v>黄香菇</v>
@@ -2009,28 +2009,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D43" t="str">
-        <v>sn -甘油 3-磷酸 锂盐SN-GLYCEROL 3-PHOSPHATE LITHIUM SALT</v>
+        <v>硫胺素焦磷酸THIAMINE PYROPHOSPHATE, =95%</v>
       </c>
       <c r="E43" t="str">
-        <v>TM210906-0391</v>
+        <v>TM220620-0304</v>
       </c>
       <c r="F43" t="str">
-        <v>94124-10MG</v>
+        <v>C8754-1G</v>
       </c>
       <c r="G43" t="str">
-        <v>10.000MG</v>
+        <v>1.000G</v>
       </c>
       <c r="H43" t="str">
-        <v>616.14</v>
+        <v>233.54</v>
       </c>
       <c r="I43" t="str">
         <v>1.00</v>
       </c>
       <c r="J43" t="str">
-        <v>616.14</v>
+        <v>233.54</v>
       </c>
       <c r="K43" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L43" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202204201709004020</v>
       </c>
       <c r="B44" t="str">
         <v>黄香菇</v>
@@ -2050,7 +2050,7 @@
         <v>硫胺素焦磷酸THIAMINE PYROPHOSPHATE, =95%</v>
       </c>
       <c r="E44" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220620-0301</v>
       </c>
       <c r="F44" t="str">
         <v>C8754-1G</v>
@@ -2059,13 +2059,13 @@
         <v>1.000G</v>
       </c>
       <c r="H44" t="str">
-        <v>208.78</v>
+        <v>233.54</v>
       </c>
       <c r="I44" t="str">
         <v>1.00</v>
       </c>
       <c r="J44" t="str">
-        <v>208.78</v>
+        <v>233.54</v>
       </c>
       <c r="K44" t="str">
         <v>G</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206271628494014</v>
       </c>
       <c r="B45" t="str">
         <v>黄香菇</v>
@@ -2085,28 +2085,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D45" t="str">
-        <v>尿苷-5′-二磷酸 二钠盐 水合物URIDINE 5-DIPHOSPHATE DISODIUM S&amp;amp;</v>
+        <v>DNase I酶DNase I</v>
       </c>
       <c r="E45" t="str">
-        <v>TM210906-0405</v>
+        <v>TM220704-0376</v>
       </c>
       <c r="F45" t="str">
-        <v>94330-100MG</v>
+        <v>11284932001</v>
       </c>
       <c r="G45" t="str">
-        <v>100.000MG</v>
+        <v>100mg</v>
       </c>
       <c r="H45" t="str">
-        <v>850.14</v>
+        <v>1638.61</v>
       </c>
       <c r="I45" t="str">
-        <v>1.00</v>
+        <v>2.00</v>
       </c>
       <c r="J45" t="str">
-        <v>850.14</v>
+        <v>3277.22</v>
       </c>
       <c r="K45" t="str">
-        <v>MG</v>
+        <v>EA</v>
       </c>
       <c r="L45" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206271628494014</v>
       </c>
       <c r="B46" t="str">
         <v>黄香菇</v>
@@ -2123,28 +2123,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D46" t="str">
-        <v>尿苷5-单磷酸URIDINE 5-MONOPHOSPHATE, =98%</v>
+        <v>明胶 来源于冷水鱼类的皮肤GELATIN FROM COLD WATER FISH SKIN</v>
       </c>
       <c r="E46" t="str">
-        <v>TM210902-0344</v>
+        <v>TM220704-0375</v>
       </c>
       <c r="F46" t="str">
-        <v>U1752-1G</v>
+        <v>G7765-1L</v>
       </c>
       <c r="G46" t="str">
-        <v>1.000G</v>
+        <v>1.000KG</v>
       </c>
       <c r="H46" t="str">
-        <v>1517.31</v>
+        <v>1555.04</v>
       </c>
       <c r="I46" t="str">
-        <v>1.00</v>
+        <v>3.00</v>
       </c>
       <c r="J46" t="str">
-        <v>1517.31</v>
+        <v>4665.12</v>
       </c>
       <c r="K46" t="str">
-        <v>G</v>
+        <v>L</v>
       </c>
       <c r="L46" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206271628494014</v>
       </c>
       <c r="B47" t="str">
         <v>黄香菇</v>
@@ -2161,25 +2161,25 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D47" t="str">
-        <v>甜菜碱BETAINE FREE BASE ANHYDROUS</v>
+        <v>L -赖氨酸L-LYSINE, = 98% (TLC)</v>
       </c>
       <c r="E47" t="str">
-        <v>TM210906-0391</v>
+        <v>TM220704-0382</v>
       </c>
       <c r="F47" t="str">
-        <v>B2629-50G</v>
+        <v>L5501-25G</v>
       </c>
       <c r="G47" t="str">
-        <v>50.000G</v>
+        <v>25.000G</v>
       </c>
       <c r="H47" t="str">
-        <v>314.24</v>
+        <v>1085.86</v>
       </c>
       <c r="I47" t="str">
         <v>1.00</v>
       </c>
       <c r="J47" t="str">
-        <v>314.24</v>
+        <v>1085.86</v>
       </c>
       <c r="K47" t="str">
         <v>G</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202206271628494014</v>
       </c>
       <c r="B48" t="str">
         <v>黄香菇</v>
@@ -2199,28 +2199,28 @@
         <v>RG00901-夏宁邵</v>
       </c>
       <c r="D48" t="str">
-        <v>CYTIDINE 5-MONOPHOSPHATE DISODIUM&amp;amp;</v>
+        <v>MES, LOW MOISTURE CONTENT</v>
       </c>
       <c r="E48" t="str">
-        <v>TM210906-0391</v>
+        <v>TM220704-0373</v>
       </c>
       <c r="F48" t="str">
-        <v>C1006-500MG</v>
+        <v>M3671-250G</v>
       </c>
       <c r="G48" t="str">
-        <v>500.000MG</v>
+        <v>250.000G</v>
       </c>
       <c r="H48" t="str">
-        <v>349.75</v>
+        <v>3820.03</v>
       </c>
       <c r="I48" t="str">
         <v>1.00</v>
       </c>
       <c r="J48" t="str">
-        <v>349.75</v>
+        <v>3820.03</v>
       </c>
       <c r="K48" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L48" t="str">
         <v>现货一周内，期货咨询销售</v>
@@ -2228,990 +2228,40 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>PO202108251027264010</v>
+        <v>PO202207011544370212</v>
       </c>
       <c r="B49" t="str">
-        <v>黄香菇</v>
+        <v>王国良</v>
       </c>
       <c r="C49" t="str">
-        <v>RG00901-夏宁邵</v>
+        <v>RG01833-王国良</v>
       </c>
       <c r="D49" t="str">
-        <v>羟脯氨酸HYDROXYPROLINE</v>
+        <v>泰莫西芬TAMOXIFEN FREE BASE</v>
       </c>
       <c r="E49" t="str">
-        <v>TM210906-0389</v>
+        <v>TM220705-0109</v>
       </c>
       <c r="F49" t="str">
-        <v>PHR1939-500MG</v>
+        <v>T5648-1G</v>
       </c>
       <c r="G49" t="str">
-        <v>500.000MG</v>
+        <v>1.000G</v>
       </c>
       <c r="H49" t="str">
-        <v>1393.68</v>
+        <v>2608.67</v>
       </c>
       <c r="I49" t="str">
         <v>1.00</v>
       </c>
       <c r="J49" t="str">
-        <v>1393.68</v>
+        <v>2608.67</v>
       </c>
       <c r="K49" t="str">
-        <v>MG</v>
+        <v>G</v>
       </c>
       <c r="L49" t="str">
         <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B50" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C50" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D50" t="str">
-        <v>烟酸NICOTINIC ACID</v>
-      </c>
-      <c r="E50" t="str">
-        <v>TM210906-0389</v>
-      </c>
-      <c r="F50" t="str">
-        <v>72309-100G</v>
-      </c>
-      <c r="G50" t="str">
-        <v>100.000G</v>
-      </c>
-      <c r="H50" t="str">
-        <v>373.43</v>
-      </c>
-      <c r="I50" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J50" t="str">
-        <v>373.43</v>
-      </c>
-      <c r="K50" t="str">
-        <v>G</v>
-      </c>
-      <c r="L50" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B51" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C51" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D51" t="str">
-        <v>β-烟酰胺单核苷酸B-NICOTINAMIDE MONONUCLEOTIDE</v>
-      </c>
-      <c r="E51" t="str">
-        <v>TM210906-0391</v>
-      </c>
-      <c r="F51" t="str">
-        <v>N3501-25MG</v>
-      </c>
-      <c r="G51" t="str">
-        <v>25.000MG</v>
-      </c>
-      <c r="H51" t="str">
-        <v>937.30</v>
-      </c>
-      <c r="I51" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J51" t="str">
-        <v>937.30</v>
-      </c>
-      <c r="K51" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L51" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B52" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C52" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D52" t="str">
-        <v>叶酸FOLIC ACID</v>
-      </c>
-      <c r="E52" t="str">
-        <v>TM210906-0391</v>
-      </c>
-      <c r="F52" t="str">
-        <v>F7876-1G</v>
-      </c>
-      <c r="G52" t="str">
-        <v>1.000G</v>
-      </c>
-      <c r="H52" t="str">
-        <v>168.86</v>
-      </c>
-      <c r="I52" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J52" t="str">
-        <v>168.86</v>
-      </c>
-      <c r="K52" t="str">
-        <v>G</v>
-      </c>
-      <c r="L52" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B53" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C53" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D53" t="str">
-        <v>二氢叶酸DIHYDROFOLIC ACID</v>
-      </c>
-      <c r="E53" t="str">
-        <v>TM210906-0391</v>
-      </c>
-      <c r="F53" t="str">
-        <v>D7006-10MG</v>
-      </c>
-      <c r="G53" t="str">
-        <v>10.000MG</v>
-      </c>
-      <c r="H53" t="str">
-        <v>855.09</v>
-      </c>
-      <c r="I53" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J53" t="str">
-        <v>855.09</v>
-      </c>
-      <c r="K53" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L53" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B54" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C54" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D54" t="str">
-        <v>四氢叶酸TETRAHYDROFOLIC ACID SEALED AMPULE</v>
-      </c>
-      <c r="E54" t="str">
-        <v>TM210906-0389</v>
-      </c>
-      <c r="F54" t="str">
-        <v>T3125-25MG</v>
-      </c>
-      <c r="G54" t="str">
-        <v>25.000MG</v>
-      </c>
-      <c r="H54" t="str">
-        <v>464.90</v>
-      </c>
-      <c r="I54" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J54" t="str">
-        <v>464.90</v>
-      </c>
-      <c r="K54" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L54" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B55" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C55" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D55" t="str">
-        <v>氨基葡萄糖GLUCOSAMINE HYDROCHLORIDE</v>
-      </c>
-      <c r="E55" t="str">
-        <v>TM210906-0389</v>
-      </c>
-      <c r="F55" t="str">
-        <v>PHR1199-500MG</v>
-      </c>
-      <c r="G55" t="str">
-        <v>500.000MG</v>
-      </c>
-      <c r="H55" t="str">
-        <v>792.52</v>
-      </c>
-      <c r="I55" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J55" t="str">
-        <v>792.52</v>
-      </c>
-      <c r="K55" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L55" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>PO202108251027264010</v>
-      </c>
-      <c r="B56" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C56" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D56" t="str">
-        <v>N -乙酰基- D -氨基葡萄糖N-ACETYL-D-GLUCOSAMINE =&amp;amp;</v>
-      </c>
-      <c r="E56" t="str">
-        <v>TM210906-0389</v>
-      </c>
-      <c r="F56" t="str">
-        <v>A8625-10MG</v>
-      </c>
-      <c r="G56" t="str">
-        <v>10.000MG</v>
-      </c>
-      <c r="H56" t="str">
-        <v>211.09</v>
-      </c>
-      <c r="I56" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J56" t="str">
-        <v>211.09</v>
-      </c>
-      <c r="K56" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L56" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B57" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C57" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D57" t="str">
-        <v>N-乙酰神经氨酸N-ACETYLNEURAMINIC ACID, SYNTHETIC</v>
-      </c>
-      <c r="E57" t="str">
-        <v>TM210819-0076</v>
-      </c>
-      <c r="F57" t="str">
-        <v>A0812-25MG</v>
-      </c>
-      <c r="G57" t="str">
-        <v>25.000MG</v>
-      </c>
-      <c r="H57" t="str">
-        <v>473.02</v>
-      </c>
-      <c r="I57" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J57" t="str">
-        <v>473.02</v>
-      </c>
-      <c r="K57" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L57" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B58" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C58" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D58" t="str">
-        <v>胞苷-5 &amp;amp; # 8242;-单磷氮乙酰神经氨酸 钠盐CYTIDINE 5-MONOPHOSPHO-N-             &amp;amp;</v>
-      </c>
-      <c r="E58" t="str">
-        <v>TM210819-0076</v>
-      </c>
-      <c r="F58" t="str">
-        <v>C8271-1MG</v>
-      </c>
-      <c r="G58" t="str">
-        <v>1.000MG</v>
-      </c>
-      <c r="H58" t="str">
-        <v>673.66</v>
-      </c>
-      <c r="I58" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J58" t="str">
-        <v>673.66</v>
-      </c>
-      <c r="K58" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L58" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B59" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C59" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D59" t="str">
-        <v>D -(+)-半乳糖D-(+)-GALACTOSE, = 99%</v>
-      </c>
-      <c r="E59" t="str">
-        <v>TM210819-0076</v>
-      </c>
-      <c r="F59" t="str">
-        <v>G0750-10MG</v>
-      </c>
-      <c r="G59" t="str">
-        <v>10.000MG</v>
-      </c>
-      <c r="H59" t="str">
-        <v>192.68</v>
-      </c>
-      <c r="I59" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J59" t="str">
-        <v>192.68</v>
-      </c>
-      <c r="K59" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L59" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B60" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C60" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D60" t="str">
-        <v>D-MANNITOL 1-PHOSPHATE LITHIUM SALT</v>
-      </c>
-      <c r="E60" t="str">
-        <v>TM210819-0076</v>
-      </c>
-      <c r="F60" t="str">
-        <v>92416-10MG</v>
-      </c>
-      <c r="G60" t="str">
-        <v>0.010G</v>
-      </c>
-      <c r="H60" t="str">
-        <v>4606.16</v>
-      </c>
-      <c r="I60" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J60" t="str">
-        <v>4606.16</v>
-      </c>
-      <c r="K60" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L60" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B61" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C61" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D61" t="str">
-        <v>4-羟肉桂酸for synthesis</v>
-      </c>
-      <c r="E61" t="str">
-        <v>TM210906-0388</v>
-      </c>
-      <c r="F61" t="str">
-        <v>8002370010</v>
-      </c>
-      <c r="G61" t="str">
-        <v>1EA</v>
-      </c>
-      <c r="H61" t="str">
-        <v>350.60</v>
-      </c>
-      <c r="I61" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J61" t="str">
-        <v>350.60</v>
-      </c>
-      <c r="K61" t="str">
-        <v>EA</v>
-      </c>
-      <c r="L61" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B62" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C62" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D62" t="str">
-        <v>吲哚-3-丙酮酸INDOLE-3-PYRUVIC ACID, =97%</v>
-      </c>
-      <c r="E62" t="str">
-        <v>TM210819-0079</v>
-      </c>
-      <c r="F62" t="str">
-        <v>I7017-1G</v>
-      </c>
-      <c r="G62" t="str">
-        <v>1.000G</v>
-      </c>
-      <c r="H62" t="str">
-        <v>1640.14</v>
-      </c>
-      <c r="I62" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J62" t="str">
-        <v>1640.14</v>
-      </c>
-      <c r="K62" t="str">
-        <v>G</v>
-      </c>
-      <c r="L62" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="str">
-        <v>PO202108251044194018</v>
-      </c>
-      <c r="B63" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C63" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D63" t="str">
-        <v>6-磷酸葡萄糖酸 三钠盐6-PHOSPHOGLUCONIC ACID TRISODIUM SALT &amp;amp;&amp;amp;</v>
-      </c>
-      <c r="E63" t="str">
-        <v>TM210906-0393</v>
-      </c>
-      <c r="F63" t="str">
-        <v>P7877-100MG</v>
-      </c>
-      <c r="G63" t="str">
-        <v>100.000MG</v>
-      </c>
-      <c r="H63" t="str">
-        <v>402.66</v>
-      </c>
-      <c r="I63" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J63" t="str">
-        <v>402.66</v>
-      </c>
-      <c r="K63" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L63" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>PO202108171046304011</v>
-      </c>
-      <c r="B64" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C64" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D64" t="str">
-        <v>花生四烯酸ARACHIDONIC ACID, 95.0% GC</v>
-      </c>
-      <c r="E64" t="str">
-        <v>TM210819-0079</v>
-      </c>
-      <c r="F64" t="str">
-        <v>10931-250MG</v>
-      </c>
-      <c r="G64" t="str">
-        <v>250.000MG</v>
-      </c>
-      <c r="H64" t="str">
-        <v>1373.80</v>
-      </c>
-      <c r="I64" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J64" t="str">
-        <v>1373.80</v>
-      </c>
-      <c r="K64" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L64" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B65" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C65" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D65" t="str">
-        <v>羟乙基哌嗪乙硫磺酸HEPES</v>
-      </c>
-      <c r="E65" t="str">
-        <v>TM210906-0430</v>
-      </c>
-      <c r="F65" t="str">
-        <v>H3375-1KG</v>
-      </c>
-      <c r="G65" t="str">
-        <v>1.000KG</v>
-      </c>
-      <c r="H65" t="str">
-        <v>5389.99</v>
-      </c>
-      <c r="I65" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J65" t="str">
-        <v>5389.99</v>
-      </c>
-      <c r="K65" t="str">
-        <v>KG</v>
-      </c>
-      <c r="L65" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B66" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C66" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D66" t="str">
-        <v>IGEPAL CA 630</v>
-      </c>
-      <c r="E66" t="str">
-        <v>TM210906-0430</v>
-      </c>
-      <c r="F66" t="str">
-        <v>I3021-100ML</v>
-      </c>
-      <c r="G66" t="str">
-        <v>106.000G</v>
-      </c>
-      <c r="H66" t="str">
-        <v>545.89</v>
-      </c>
-      <c r="I66" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J66" t="str">
-        <v>545.89</v>
-      </c>
-      <c r="K66" t="str">
-        <v>ML</v>
-      </c>
-      <c r="L66" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B67" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C67" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D67" t="str">
-        <v>6-(马来酰亚胺基)己酸琥珀酰亚胺酯EPISILON-MALEIMIDOCAPROIC ACID N- HYDROX</v>
-      </c>
-      <c r="E67" t="str">
-        <v>TM210906-0430</v>
-      </c>
-      <c r="F67" t="str">
-        <v>M9794-100MG</v>
-      </c>
-      <c r="G67" t="str">
-        <v>100.000MG</v>
-      </c>
-      <c r="H67" t="str">
-        <v>4502.29</v>
-      </c>
-      <c r="I67" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J67" t="str">
-        <v>4502.29</v>
-      </c>
-      <c r="K67" t="str">
-        <v>MG</v>
-      </c>
-      <c r="L67" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B68" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C68" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D68" t="str">
-        <v>硼烷吡啶络合物BORANE-PYRIDINE COMPLEX</v>
-      </c>
-      <c r="E68" t="str">
-        <v>TM210906-0424</v>
-      </c>
-      <c r="F68" t="str">
-        <v>179752-5G</v>
-      </c>
-      <c r="G68" t="str">
-        <v>5.000G</v>
-      </c>
-      <c r="H68" t="str">
-        <v>321.91</v>
-      </c>
-      <c r="I68" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J68" t="str">
-        <v>321.91</v>
-      </c>
-      <c r="K68" t="str">
-        <v>G</v>
-      </c>
-      <c r="L68" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B69" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C69" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D69" t="str">
-        <v>ANTI-OTUB2</v>
-      </c>
-      <c r="E69" t="str">
-        <v>TM210906-0424</v>
-      </c>
-      <c r="F69" t="str">
-        <v>HPA002329-100UL</v>
-      </c>
-      <c r="G69" t="str">
-        <v>100.000MG</v>
-      </c>
-      <c r="H69" t="str">
-        <v>3512.39</v>
-      </c>
-      <c r="I69" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J69" t="str">
-        <v>3512.39</v>
-      </c>
-      <c r="K69" t="str">
-        <v>μL</v>
-      </c>
-      <c r="L69" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B70" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C70" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D70" t="str">
-        <v>4-(4,6-二甲氧基三嗪-2-基)-4-甲基吗啉盐酸盐4-(4,6-DIMETHOXY-1,3,5-TRIAZIN-2-YL)-4-&amp;amp;</v>
-      </c>
-      <c r="E70" t="str">
-        <v>TM210906-0424</v>
-      </c>
-      <c r="F70" t="str">
-        <v>74104-1G-F</v>
-      </c>
-      <c r="G70" t="str">
-        <v>1.000G</v>
-      </c>
-      <c r="H70" t="str">
-        <v>725.29</v>
-      </c>
-      <c r="I70" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J70" t="str">
-        <v>725.29</v>
-      </c>
-      <c r="K70" t="str">
-        <v>G</v>
-      </c>
-      <c r="L70" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B71" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C71" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D71" t="str">
-        <v>胶原酶DCollagenase D</v>
-      </c>
-      <c r="E71" t="str">
-        <v>TM210906-0424</v>
-      </c>
-      <c r="F71" t="str">
-        <v>11088866001</v>
-      </c>
-      <c r="G71" t="str">
-        <v>1EA</v>
-      </c>
-      <c r="H71" t="str">
-        <v>2396.48</v>
-      </c>
-      <c r="I71" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J71" t="str">
-        <v>2396.48</v>
-      </c>
-      <c r="K71" t="str">
-        <v>EA</v>
-      </c>
-      <c r="L71" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>PO202109061710214010</v>
-      </c>
-      <c r="B72" t="str">
-        <v>黄香菇</v>
-      </c>
-      <c r="C72" t="str">
-        <v>RG00901-夏宁邵</v>
-      </c>
-      <c r="D72" t="str">
-        <v>布安溶液</v>
-      </c>
-      <c r="E72" t="str">
-        <v>TM210906-0424</v>
-      </c>
-      <c r="F72" t="str">
-        <v>HT10132-1L</v>
-      </c>
-      <c r="G72" t="str">
-        <v>1L</v>
-      </c>
-      <c r="H72" t="str">
-        <v>761.11</v>
-      </c>
-      <c r="I72" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J72" t="str">
-        <v>761.11</v>
-      </c>
-      <c r="K72" t="str">
-        <v>瓶</v>
-      </c>
-      <c r="L72" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>PO202109231535160384</v>
-      </c>
-      <c r="B73" t="str">
-        <v>李一凡</v>
-      </c>
-      <c r="C73" t="str">
-        <v>RG01013-纪志梁</v>
-      </c>
-      <c r="D73" t="str">
-        <v>ANTI-KPNB1</v>
-      </c>
-      <c r="E73" t="str">
-        <v>TM210924-0001</v>
-      </c>
-      <c r="F73" t="str">
-        <v>HPA029878-100UL</v>
-      </c>
-      <c r="G73" t="str">
-        <v>100.000MG</v>
-      </c>
-      <c r="H73" t="str">
-        <v>3981.49</v>
-      </c>
-      <c r="I73" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J73" t="str">
-        <v>3981.49</v>
-      </c>
-      <c r="K73" t="str">
-        <v>μL</v>
-      </c>
-      <c r="L73" t="str">
-        <v>现货一周内，期货咨询销售</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>PO202109231535160384</v>
-      </c>
-      <c r="B74" t="str">
-        <v>李一凡</v>
-      </c>
-      <c r="C74" t="str">
-        <v>RG01013-纪志梁</v>
-      </c>
-      <c r="D74" t="str">
-        <v>Monoclonal Anti-Importin 4 antibody produced in rat</v>
-      </c>
-      <c r="E74" t="str">
-        <v>TM210924-0001</v>
-      </c>
-      <c r="F74" t="str">
-        <v>SAB4200192-25UL</v>
-      </c>
-      <c r="G74" t="str">
-        <v>25UL</v>
-      </c>
-      <c r="H74" t="str">
-        <v>655.28</v>
-      </c>
-      <c r="I74" t="str">
-        <v>1.00</v>
-      </c>
-      <c r="J74" t="str">
-        <v>655.28</v>
-      </c>
-      <c r="K74" t="str">
-        <v>瓶</v>
-      </c>
-      <c r="L74" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>